<commit_message>
fix alignment tool output for benchmark accuracy
</commit_message>
<xml_diff>
--- a/benchmarking/coronavirus-benchmarking.xlsx
+++ b/benchmarking/coronavirus-benchmarking.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Preprocessing Query (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Searching Time (s)</t>
+    <t xml:space="preserve">Search Time (s)</t>
   </si>
   <si>
     <t xml:space="preserve">Total Time (s)</t>
@@ -55,10 +55,10 @@
     <t xml:space="preserve">BLAST</t>
   </si>
   <si>
-    <t xml:space="preserve">DIAMOND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMseqs2</t>
+    <t xml:space="preserve">* DIAMOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* MMseqs2</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -310,7 +310,7 @@
         <v>6.427</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>